<commit_message>
upadated code to close files
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC03_CCDI_RowDataValidation_phs003111.xlsx
+++ b/InputFiles/CCDI/TC03_CCDI_RowDataValidation_phs003111.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C8585E-8FA4-4245-94C7-F37AEEDAB269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A0B763-2271-4868-9C67-57070D932534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -320,7 +320,7 @@
 sm.sample_id AS `Sample ID`,
 file.dcf_indexd_guid AS `GUID`,
 file.md5sum AS `MD5sum`
-Order by `File Name`</t>
+Order by `File Name`desc</t>
   </si>
 </sst>
 </file>
@@ -692,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>